<commit_message>
[monitoring_hard_drop] Update figure colors to be consistent.
</commit_message>
<xml_diff>
--- a/monitoring_wcet/figs_src/monitoring_pipeline.xlsx
+++ b/monitoring_wcet/figs_src/monitoring_pipeline.xlsx
@@ -96,7 +96,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF7C80"/>
+        <fgColor rgb="FFFB9A99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,25 +269,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -303,6 +291,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -313,6 +313,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE31A1C"/>
+      <color rgb="FFFB9A99"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FF66FFFF"/>
@@ -617,7 +619,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -672,113 +674,113 @@
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="18"/>
+      <c r="H5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="10"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:11" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="12"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="13">
         <v>2</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="13">
         <v>0</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <v>0</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="13">
         <v>0</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="14">
         <v>0</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>0</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="13">
         <v>0</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="15">
         <v>0</v>
       </c>
     </row>

</xml_diff>